<commit_message>
metrics and json support added to SourceCode.php. Improved summary and frequencies management in Structures.php
</commit_message>
<xml_diff>
--- a/tests/data/input/Symbols.xlsx
+++ b/tests/data/input/Symbols.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="270" windowWidth="21675" windowHeight="12015"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="18030" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1215,6 +1216,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>